<commit_message>
Committed By Avanica.Made Changes in Change scenarios.
MaterialChangeScript.java
Material_Change_Page.java

Changed Dataprovider to match with change flow.
Base UOM fix by scrolling
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mendix_Workspace\Mendix\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git\Mendix\Mendix\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D37A699-87B6-459E-8A02-290D83DFED7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB17E2E2-30A3-40D1-97B1-8A38462E4410}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="82">
   <si>
     <t>S.NO</t>
   </si>
@@ -259,13 +259,22 @@
   </si>
   <si>
     <t>LDS</t>
+  </si>
+  <si>
+    <t>ChangeMaterial_Nav</t>
+  </si>
+  <si>
+    <t>ChangeMaterial_Reject_Discard</t>
+  </si>
+  <si>
+    <t>1402111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Mic Shell Dlg"/>
@@ -273,6 +282,12 @@
     <font>
       <sz val="11"/>
       <name val="Mic Shell Dlg"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -306,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -314,6 +329,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,32 +677,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IX4"/>
+  <dimension ref="A1:IX6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="1" customWidth="1"/>
-    <col min="17" max="258" width="9.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" style="1" customWidth="1"/>
+    <col min="17" max="258" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.75" customHeight="1">
+    <row r="1" spans="1:258" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +752,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1">
+    <row r="2" spans="1:258" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -739,7 +763,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>16</v>
@@ -772,7 +796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1">
+    <row r="3" spans="1:258" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -819,7 +843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1">
+    <row r="4" spans="1:258" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -866,9 +890,344 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:258" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="2">
+        <v>161144</v>
+      </c>
+      <c r="L5" s="2">
+        <v>30007590</v>
+      </c>
+      <c r="M5" s="2">
+        <v>30007783</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:258" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="10">
+        <v>30007590</v>
+      </c>
+      <c r="M6" s="10">
+        <v>30007783</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+      <c r="AX6" s="9"/>
+      <c r="AY6" s="9"/>
+      <c r="AZ6" s="9"/>
+      <c r="BA6" s="9"/>
+      <c r="BB6" s="9"/>
+      <c r="BC6" s="9"/>
+      <c r="BD6" s="9"/>
+      <c r="BE6" s="9"/>
+      <c r="BF6" s="9"/>
+      <c r="BG6" s="9"/>
+      <c r="BH6" s="9"/>
+      <c r="BI6" s="9"/>
+      <c r="BJ6" s="9"/>
+      <c r="BK6" s="9"/>
+      <c r="BL6" s="9"/>
+      <c r="BM6" s="9"/>
+      <c r="BN6" s="9"/>
+      <c r="BO6" s="9"/>
+      <c r="BP6" s="9"/>
+      <c r="BQ6" s="9"/>
+      <c r="BR6" s="9"/>
+      <c r="BS6" s="9"/>
+      <c r="BT6" s="9"/>
+      <c r="BU6" s="9"/>
+      <c r="BV6" s="9"/>
+      <c r="BW6" s="9"/>
+      <c r="BX6" s="9"/>
+      <c r="BY6" s="9"/>
+      <c r="BZ6" s="9"/>
+      <c r="CA6" s="9"/>
+      <c r="CB6" s="9"/>
+      <c r="CC6" s="9"/>
+      <c r="CD6" s="9"/>
+      <c r="CE6" s="9"/>
+      <c r="CF6" s="9"/>
+      <c r="CG6" s="9"/>
+      <c r="CH6" s="9"/>
+      <c r="CI6" s="9"/>
+      <c r="CJ6" s="9"/>
+      <c r="CK6" s="9"/>
+      <c r="CL6" s="9"/>
+      <c r="CM6" s="9"/>
+      <c r="CN6" s="9"/>
+      <c r="CO6" s="9"/>
+      <c r="CP6" s="9"/>
+      <c r="CQ6" s="9"/>
+      <c r="CR6" s="9"/>
+      <c r="CS6" s="9"/>
+      <c r="CT6" s="9"/>
+      <c r="CU6" s="9"/>
+      <c r="CV6" s="9"/>
+      <c r="CW6" s="9"/>
+      <c r="CX6" s="9"/>
+      <c r="CY6" s="9"/>
+      <c r="CZ6" s="9"/>
+      <c r="DA6" s="9"/>
+      <c r="DB6" s="9"/>
+      <c r="DC6" s="9"/>
+      <c r="DD6" s="9"/>
+      <c r="DE6" s="9"/>
+      <c r="DF6" s="9"/>
+      <c r="DG6" s="9"/>
+      <c r="DH6" s="9"/>
+      <c r="DI6" s="9"/>
+      <c r="DJ6" s="9"/>
+      <c r="DK6" s="9"/>
+      <c r="DL6" s="9"/>
+      <c r="DM6" s="9"/>
+      <c r="DN6" s="9"/>
+      <c r="DO6" s="9"/>
+      <c r="DP6" s="9"/>
+      <c r="DQ6" s="9"/>
+      <c r="DR6" s="9"/>
+      <c r="DS6" s="9"/>
+      <c r="DT6" s="9"/>
+      <c r="DU6" s="9"/>
+      <c r="DV6" s="9"/>
+      <c r="DW6" s="9"/>
+      <c r="DX6" s="9"/>
+      <c r="DY6" s="9"/>
+      <c r="DZ6" s="9"/>
+      <c r="EA6" s="9"/>
+      <c r="EB6" s="9"/>
+      <c r="EC6" s="9"/>
+      <c r="ED6" s="9"/>
+      <c r="EE6" s="9"/>
+      <c r="EF6" s="9"/>
+      <c r="EG6" s="9"/>
+      <c r="EH6" s="9"/>
+      <c r="EI6" s="9"/>
+      <c r="EJ6" s="9"/>
+      <c r="EK6" s="9"/>
+      <c r="EL6" s="9"/>
+      <c r="EM6" s="9"/>
+      <c r="EN6" s="9"/>
+      <c r="EO6" s="9"/>
+      <c r="EP6" s="9"/>
+      <c r="EQ6" s="9"/>
+      <c r="ER6" s="9"/>
+      <c r="ES6" s="9"/>
+      <c r="ET6" s="9"/>
+      <c r="EU6" s="9"/>
+      <c r="EV6" s="9"/>
+      <c r="EW6" s="9"/>
+      <c r="EX6" s="9"/>
+      <c r="EY6" s="9"/>
+      <c r="EZ6" s="9"/>
+      <c r="FA6" s="9"/>
+      <c r="FB6" s="9"/>
+      <c r="FC6" s="9"/>
+      <c r="FD6" s="9"/>
+      <c r="FE6" s="9"/>
+      <c r="FF6" s="9"/>
+      <c r="FG6" s="9"/>
+      <c r="FH6" s="9"/>
+      <c r="FI6" s="9"/>
+      <c r="FJ6" s="9"/>
+      <c r="FK6" s="9"/>
+      <c r="FL6" s="9"/>
+      <c r="FM6" s="9"/>
+      <c r="FN6" s="9"/>
+      <c r="FO6" s="9"/>
+      <c r="FP6" s="9"/>
+      <c r="FQ6" s="9"/>
+      <c r="FR6" s="9"/>
+      <c r="FS6" s="9"/>
+      <c r="FT6" s="9"/>
+      <c r="FU6" s="9"/>
+      <c r="FV6" s="9"/>
+      <c r="FW6" s="9"/>
+      <c r="FX6" s="9"/>
+      <c r="FY6" s="9"/>
+      <c r="FZ6" s="9"/>
+      <c r="GA6" s="9"/>
+      <c r="GB6" s="9"/>
+      <c r="GC6" s="9"/>
+      <c r="GD6" s="9"/>
+      <c r="GE6" s="9"/>
+      <c r="GF6" s="9"/>
+      <c r="GG6" s="9"/>
+      <c r="GH6" s="9"/>
+      <c r="GI6" s="9"/>
+      <c r="GJ6" s="9"/>
+      <c r="GK6" s="9"/>
+      <c r="GL6" s="9"/>
+      <c r="GM6" s="9"/>
+      <c r="GN6" s="9"/>
+      <c r="GO6" s="9"/>
+      <c r="GP6" s="9"/>
+      <c r="GQ6" s="9"/>
+      <c r="GR6" s="9"/>
+      <c r="GS6" s="9"/>
+      <c r="GT6" s="9"/>
+      <c r="GU6" s="9"/>
+      <c r="GV6" s="9"/>
+      <c r="GW6" s="9"/>
+      <c r="GX6" s="9"/>
+      <c r="GY6" s="9"/>
+      <c r="GZ6" s="9"/>
+      <c r="HA6" s="9"/>
+      <c r="HB6" s="9"/>
+      <c r="HC6" s="9"/>
+      <c r="HD6" s="9"/>
+      <c r="HE6" s="9"/>
+      <c r="HF6" s="9"/>
+      <c r="HG6" s="9"/>
+      <c r="HH6" s="9"/>
+      <c r="HI6" s="9"/>
+      <c r="HJ6" s="9"/>
+      <c r="HK6" s="9"/>
+      <c r="HL6" s="9"/>
+      <c r="HM6" s="9"/>
+      <c r="HN6" s="9"/>
+      <c r="HO6" s="9"/>
+      <c r="HP6" s="9"/>
+      <c r="HQ6" s="9"/>
+      <c r="HR6" s="9"/>
+      <c r="HS6" s="9"/>
+      <c r="HT6" s="9"/>
+      <c r="HU6" s="9"/>
+      <c r="HV6" s="9"/>
+      <c r="HW6" s="9"/>
+      <c r="HX6" s="9"/>
+      <c r="HY6" s="9"/>
+      <c r="HZ6" s="9"/>
+      <c r="IA6" s="9"/>
+      <c r="IB6" s="9"/>
+      <c r="IC6" s="9"/>
+      <c r="ID6" s="9"/>
+      <c r="IE6" s="9"/>
+      <c r="IF6" s="9"/>
+      <c r="IG6" s="9"/>
+      <c r="IH6" s="9"/>
+      <c r="II6" s="9"/>
+      <c r="IJ6" s="9"/>
+      <c r="IK6" s="9"/>
+      <c r="IL6" s="9"/>
+      <c r="IM6" s="9"/>
+      <c r="IN6" s="9"/>
+      <c r="IO6" s="9"/>
+      <c r="IP6" s="9"/>
+      <c r="IQ6" s="9"/>
+      <c r="IR6" s="9"/>
+      <c r="IS6" s="9"/>
+      <c r="IT6" s="9"/>
+      <c r="IU6" s="9"/>
+      <c r="IV6" s="9"/>
+      <c r="IW6" s="9"/>
+      <c r="IX6" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -885,19 +1244,19 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="55" style="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="55" style="1" customWidth="1"/>
-    <col min="6" max="254" width="9.140625" style="1" customWidth="1"/>
-    <col min="255" max="255" width="4.85546875" style="1" customWidth="1"/>
+    <col min="6" max="254" width="9.109375" style="1" customWidth="1"/>
+    <col min="255" max="255" width="4.88671875" style="1" customWidth="1"/>
     <col min="256" max="256" width="55" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1">
+    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -914,7 +1273,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -931,7 +1290,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -948,7 +1307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -965,7 +1324,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -982,7 +1341,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -1018,14 +1377,14 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="123.140625" style="3" customWidth="1"/>
-    <col min="3" max="256" width="9.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="123.109375" style="3" customWidth="1"/>
+    <col min="3" max="256" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.75" customHeight="1">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -1033,7 +1392,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -1041,7 +1400,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1049,7 +1408,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1057,7 +1416,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1065,7 +1424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1073,7 +1432,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1081,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1089,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -1097,7 +1456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -1105,7 +1464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -1113,7 +1472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -1121,7 +1480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -1129,7 +1488,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1137,7 +1496,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1145,7 +1504,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -1153,7 +1512,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1161,7 +1520,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
@@ -1169,7 +1528,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -1177,7 +1536,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -1185,7 +1544,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Added change material reject with discard scenario
</commit_message>
<xml_diff>
--- a/Mendix/input/Mendix_TestPlan.xlsx
+++ b/Mendix/input/Mendix_TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git\Mendix\Mendix\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB17E2E2-30A3-40D1-97B1-8A38462E4410}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A1CA3C-6FDC-471D-AE98-A68915E2F279}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="84">
   <si>
     <t>S.NO</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Production | Raw material, ingredient or processing aid</t>
   </si>
   <si>
-    <t>Create_Material</t>
-  </si>
-  <si>
     <t>Create_Material_Draft</t>
   </si>
   <si>
@@ -267,7 +264,16 @@
     <t>ChangeMaterial_Reject_Discard</t>
   </si>
   <si>
-    <t>1402111</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>CreateMaterial</t>
+  </si>
+  <si>
+    <t>1405328</t>
+  </si>
+  <si>
+    <t>410086</t>
   </si>
 </sst>
 </file>
@@ -677,7 +683,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IX6"/>
+  <dimension ref="A1:IX7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
@@ -688,12 +694,13 @@
     <col min="1" max="1" width="5.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="21.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="21.109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="1" customWidth="1"/>
@@ -707,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -719,16 +726,16 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -760,7 +767,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
@@ -775,10 +782,10 @@
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
@@ -804,7 +811,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -819,10 +826,10 @@
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
@@ -848,10 +855,10 @@
         <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>19</v>
@@ -866,10 +873,10 @@
         <v>5</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>15</v>
@@ -895,10 +902,10 @@
         <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -913,10 +920,10 @@
         <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>15</v>
@@ -945,13 +952,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>81</v>
+      <c r="E6" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>4</v>
@@ -960,15 +967,17 @@
         <v>5</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="L6" s="10">
         <v>30007590</v>
       </c>
@@ -1225,6 +1234,20 @@
       <c r="IW6" s="9"/>
       <c r="IX6" s="9"/>
     </row>
+    <row r="7" spans="1:258" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>